<commit_message>
Construção de uma AI
</commit_message>
<xml_diff>
--- a/Atumação_web/Preços_Produtos_atualizados.xlsx
+++ b/Atumação_web/Preços_Produtos_atualizados.xlsx
@@ -462,16 +462,16 @@
         <v>14</v>
       </c>
       <c r="D2">
-        <v>5.523499999999999</v>
+        <v>5.5322</v>
       </c>
       <c r="E2">
-        <v>5523.444764999999</v>
+        <v>5532.144678</v>
       </c>
       <c r="F2">
         <v>1.4</v>
       </c>
       <c r="G2">
-        <v>7732.823</v>
+        <v>7745.003</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -485,16 +485,16 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>6.331637761000001</v>
+        <v>6.336443575000001</v>
       </c>
       <c r="E3">
-        <v>28492.3699245</v>
+        <v>28513.9960875</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3">
-        <v>56984.74</v>
+        <v>57027.992</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -508,16 +508,16 @@
         <v>14</v>
       </c>
       <c r="D4">
-        <v>5.523499999999999</v>
+        <v>5.5322</v>
       </c>
       <c r="E4">
-        <v>4971.094765</v>
+        <v>4978.924677999999</v>
       </c>
       <c r="F4">
         <v>1.7</v>
       </c>
       <c r="G4">
-        <v>8450.861000000001</v>
+        <v>8464.172</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -531,16 +531,16 @@
         <v>14</v>
       </c>
       <c r="D5">
-        <v>5.523499999999999</v>
+        <v>5.5322</v>
       </c>
       <c r="E5">
-        <v>4413.2765</v>
+        <v>4420.2278</v>
       </c>
       <c r="F5">
         <v>1.7</v>
       </c>
       <c r="G5">
-        <v>7502.57</v>
+        <v>7514.387</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -554,16 +554,16 @@
         <v>15</v>
       </c>
       <c r="D6">
-        <v>6.331637761000001</v>
+        <v>6.336443575000001</v>
       </c>
       <c r="E6">
-        <v>18994.913283</v>
+        <v>19009.330725</v>
       </c>
       <c r="F6">
         <v>1.9</v>
       </c>
       <c r="G6">
-        <v>36090.335</v>
+        <v>36117.728</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -577,16 +577,16 @@
         <v>14</v>
       </c>
       <c r="D7">
-        <v>5.523499999999999</v>
+        <v>5.5322</v>
       </c>
       <c r="E7">
-        <v>2653.93128</v>
+        <v>2658.111456</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7">
-        <v>5307.863</v>
+        <v>5316.223</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -600,16 +600,16 @@
         <v>16</v>
       </c>
       <c r="D8">
-        <v>323.18</v>
+        <v>324.08</v>
       </c>
       <c r="E8">
-        <v>6463.6</v>
+        <v>6481.599999999999</v>
       </c>
       <c r="F8">
         <v>1.15</v>
       </c>
       <c r="G8">
-        <v>7433.14</v>
+        <v>7453.84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otimização na captura das linhas e das colunas de um DataFrame)
</commit_message>
<xml_diff>
--- a/Atumação_web/Preços_Produtos_atualizados.xlsx
+++ b/Atumação_web/Preços_Produtos_atualizados.xlsx
@@ -462,16 +462,16 @@
         <v>14</v>
       </c>
       <c r="D2">
-        <v>5.5322</v>
+        <v>5.5158</v>
       </c>
       <c r="E2">
-        <v>5532.144678</v>
+        <v>5515.744842</v>
       </c>
       <c r="F2">
         <v>1.4</v>
       </c>
       <c r="G2">
-        <v>7745.003</v>
+        <v>7722.043</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -485,16 +485,16 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>6.336443575000001</v>
+        <v>6.296031973000001</v>
       </c>
       <c r="E3">
-        <v>28513.9960875</v>
+        <v>28332.1438785</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3">
-        <v>57027.992</v>
+        <v>56664.288</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -508,16 +508,16 @@
         <v>14</v>
       </c>
       <c r="D4">
-        <v>5.5322</v>
+        <v>5.5158</v>
       </c>
       <c r="E4">
-        <v>4978.924677999999</v>
+        <v>4964.164842</v>
       </c>
       <c r="F4">
         <v>1.7</v>
       </c>
       <c r="G4">
-        <v>8464.172</v>
+        <v>8439.08</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -531,16 +531,16 @@
         <v>14</v>
       </c>
       <c r="D5">
-        <v>5.5322</v>
+        <v>5.5158</v>
       </c>
       <c r="E5">
-        <v>4420.2278</v>
+        <v>4407.124199999999</v>
       </c>
       <c r="F5">
         <v>1.7</v>
       </c>
       <c r="G5">
-        <v>7514.387</v>
+        <v>7492.111</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -554,16 +554,16 @@
         <v>15</v>
       </c>
       <c r="D6">
-        <v>6.336443575000001</v>
+        <v>6.296031973000001</v>
       </c>
       <c r="E6">
-        <v>19009.330725</v>
+        <v>18888.095919</v>
       </c>
       <c r="F6">
         <v>1.9</v>
       </c>
       <c r="G6">
-        <v>36117.728</v>
+        <v>35887.382</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -577,16 +577,16 @@
         <v>14</v>
       </c>
       <c r="D7">
-        <v>5.5322</v>
+        <v>5.5158</v>
       </c>
       <c r="E7">
-        <v>2658.111456</v>
+        <v>2650.231584</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7">
-        <v>5316.223</v>
+        <v>5300.463</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -600,16 +600,16 @@
         <v>16</v>
       </c>
       <c r="D8">
-        <v>324.08</v>
+        <v>322.39</v>
       </c>
       <c r="E8">
-        <v>6481.599999999999</v>
+        <v>6447.799999999999</v>
       </c>
       <c r="F8">
         <v>1.15</v>
       </c>
       <c r="G8">
-        <v>7453.84</v>
+        <v>7414.97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>